<commit_message>
feature: product crud update
</commit_message>
<xml_diff>
--- a/Project/Workflow.xlsx
+++ b/Project/Workflow.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Microservices Port Numbers" sheetId="1" r:id="rId1"/>
-    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
+    <sheet name="API URLS" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>Microservices</t>
   </si>
@@ -67,13 +67,61 @@
   </si>
   <si>
     <t>8080 - 8081</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>GetAll</t>
+  </si>
+  <si>
+    <t>GetById</t>
+  </si>
+  <si>
+    <t>GetByCategory</t>
+  </si>
+  <si>
+    <t>Create</t>
+  </si>
+  <si>
+    <t>Update</t>
+  </si>
+  <si>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>/products</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>METHOD</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>product</t>
+  </si>
+  <si>
+    <t>product with Id</t>
+  </si>
+  <si>
+    <t>BODY</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>nulll</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,8 +149,22 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -127,8 +189,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -216,11 +284,133 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -260,11 +450,185 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -272,6 +636,17 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="C3:E9" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
+  <tableColumns count="3">
+    <tableColumn id="1" name="METHOD" dataDxfId="3"/>
+    <tableColumn id="2" name="URL" dataDxfId="2"/>
+    <tableColumn id="3" name="BODY" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -563,8 +938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -653,13 +1028,132 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.140625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="14"/>
+    <col min="3" max="3" width="17.7109375" style="14" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" style="14" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="14" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="B2" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+    </row>
+    <row r="3" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="26"/>
+      <c r="C4" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="15" t="str">
+        <f>B3</f>
+        <v>/products</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="26"/>
+      <c r="C5" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="15" t="str">
+        <f>CONCATENATE(B3,"/id")</f>
+        <v>/products/id</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B6" s="26"/>
+      <c r="C6" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="15" t="str">
+        <f>CONCATENATE(B3,"/Category")</f>
+        <v>/products/Category</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="26"/>
+      <c r="C7" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="15" t="str">
+        <f>B3</f>
+        <v>/products</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="26"/>
+      <c r="C8" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="15" t="str">
+        <f>B3</f>
+        <v>/products</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="27"/>
+      <c r="C9" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="19" t="str">
+        <f>CONCATENATE(B3,"/id")</f>
+        <v>/products/id</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:B9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>